<commit_message>
Alteração das Regras de Negócio / Alertas.
</commit_message>
<xml_diff>
--- a/documentacao/sprint-1/requisitos.xlsx
+++ b/documentacao/sprint-1/requisitos.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\VITORIA\Data-Source\documentacao\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aluno\Desktop\VITORIA\Data-Source\documentacao\sprint-1\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="663" uniqueCount="155">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="667" uniqueCount="159">
   <si>
     <t>Histórico de alterações do documento</t>
   </si>
@@ -577,22 +577,34 @@
     <t>https://spring.io/</t>
   </si>
   <si>
-    <t>Com a indicação de x usuários, se os usuários indicados criarem uma conta, o "indicador" se tornará um usuário premium</t>
-  </si>
-  <si>
     <t>Na indicação de usuários, o usuário não pode "se auto-indicar"</t>
   </si>
   <si>
     <t>Usuários deverão ter dois tipos de perfis - premium ou free</t>
   </si>
   <si>
-    <t>Usuários premium terão privilégios que os usuários free não terão</t>
-  </si>
-  <si>
     <t>Descrição</t>
   </si>
   <si>
     <t>1.6</t>
+  </si>
+  <si>
+    <t>Pintar de amarelo o percentual de uso, caso algum componente de hardware atinja 60%</t>
+  </si>
+  <si>
+    <t>Pintar de vermelho o percentual de uso, caso algum componente de hardware atinja 75%</t>
+  </si>
+  <si>
+    <t>Alertar com um pop-up quando algum componente de hardware atingir 75%</t>
+  </si>
+  <si>
+    <t>Alertar com um pop-up quando tentarem acessar o sistema com dados de login inválidos</t>
+  </si>
+  <si>
+    <t>Com a indicação de 10 usuários, se os usuários indicados criarem uma conta, o "indicador" se tornará um usuário premium</t>
+  </si>
+  <si>
+    <t>Alertar com um pop-up caso haja problema na conexão com banco de dados - logo, problema na atualização do dashboard e/ou login</t>
   </si>
 </sst>
 </file>
@@ -852,7 +864,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="49">
+  <cellXfs count="50">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -997,6 +1009,9 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -2215,7 +2230,7 @@
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
       <pane ySplit="4" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B4" sqref="B4"/>
+      <selection pane="bottomLeft" activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="0" defaultRowHeight="12.75" zeroHeight="1" x14ac:dyDescent="0.2"/>
@@ -2339,7 +2354,7 @@
     </row>
     <row r="11" spans="2:5" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B11" s="7" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="C11" s="1" t="s">
         <v>14</v>
@@ -2540,7 +2555,7 @@
       </c>
       <c r="P2" s="45">
         <f ca="1">TODAY()</f>
-        <v>43734</v>
+        <v>43761</v>
       </c>
       <c r="R2" s="18"/>
       <c r="T2" s="31"/>
@@ -5712,7 +5727,7 @@
         <v>21</v>
       </c>
       <c r="C2" s="37" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
     </row>
     <row r="3" spans="2:3" ht="30" customHeight="1" x14ac:dyDescent="0.2">
@@ -5720,15 +5735,15 @@
         <v>1</v>
       </c>
       <c r="C3" s="38" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="4" spans="2:3" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B4" s="37">
         <v>2</v>
       </c>
-      <c r="C4" s="38" t="s">
-        <v>152</v>
+      <c r="C4" s="20" t="s">
+        <v>157</v>
       </c>
     </row>
     <row r="5" spans="2:3" ht="30" customHeight="1" x14ac:dyDescent="0.2">
@@ -5740,17 +5755,45 @@
       </c>
     </row>
     <row r="6" spans="2:3" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B6" s="37">
+      <c r="B6" s="49">
         <v>4</v>
       </c>
-      <c r="C6" s="38" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="7" spans="2:3" ht="30" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="8" spans="2:3" ht="30" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="9" spans="2:3" ht="30" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="10" spans="2:3" ht="30" customHeight="1" x14ac:dyDescent="0.2"/>
+      <c r="C6" s="26" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="7" spans="2:3" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B7" s="49">
+        <v>5</v>
+      </c>
+      <c r="C7" s="26" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="8" spans="2:3" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B8" s="49">
+        <v>6</v>
+      </c>
+      <c r="C8" s="26" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="9" spans="2:3" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B9" s="49">
+        <v>7</v>
+      </c>
+      <c r="C9" s="26" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="10" spans="2:3" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B10" s="49">
+        <v>8</v>
+      </c>
+      <c r="C10" s="26" t="s">
+        <v>158</v>
+      </c>
+    </row>
     <row r="11" spans="2:3" ht="30" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="12" spans="2:3" ht="30" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="13" spans="2:3" ht="30" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -5825,6 +5868,7 @@
     <row r="82" ht="30" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <pageSetup paperSize="0" orientation="portrait" horizontalDpi="0" verticalDpi="0" copies="0"/>
   <tableParts count="1">
     <tablePart r:id="rId1"/>
   </tableParts>

</xml_diff>